<commit_message>
login page successfuly runned
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -3,17 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1C96EB81-FE1A-4E8E-82AF-052F471E69AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{86AC9050-8644-4529-9235-71738283DB54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4B24D542-0957-4B90-AF3B-FDAF134FB36C}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="invalidlogin" sheetId="3" r:id="rId2"/>
-    <sheet name="validlogin" sheetId="2" r:id="rId3"/>
+    <sheet name="validlogin" sheetId="2" r:id="rId2"/>
+    <sheet name="register" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L13"/>
+  <oleSize ref="A1:L5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>z</t>
   </si>
@@ -40,25 +40,31 @@
     <t xml:space="preserve"> Please fill out this field </t>
   </si>
   <si>
-    <t>sdet21920@</t>
+    <t>r</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>confirmpassword</t>
+  </si>
+  <si>
+    <t>ninjalinos@work.com</t>
+  </si>
+  <si>
+    <t>sdet218920@</t>
+  </si>
+  <si>
+    <t>ninjalinos</t>
   </si>
   <si>
     <t>Invalid Username and Password</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>ninjalinos@work.com</t>
-  </si>
-  <si>
-    <t>sdet218920@</t>
-  </si>
-  <si>
-    <t>ninjalinos</t>
-  </si>
-  <si>
-    <t>ninjalinos@wrk.com</t>
+    <t>asdfew</t>
   </si>
 </sst>
 </file>
@@ -427,7 +433,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,29 +461,29 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
-        <v>3905978</v>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -486,94 +492,71 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976415C1-36FA-4E7C-B7C2-94494F85F5D9}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{DBCA3FCB-6902-42F1-816E-59BEED90B1F9}"/>
-    <hyperlink ref="A5" r:id="rId2" xr:uid="{09A66D1B-ABA8-4DD3-8D96-784BAE79E124}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{3C75CFA3-5BD8-4E60-B1B2-11E3224871F4}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{4AC1E986-F650-43F2-AF9B-852015DBA72B}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{6A9E1515-4769-4561-9686-8CA3F3AD8ECA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DB18A9-8ED1-4A2E-90AE-E21BA8F07073}">
-  <dimension ref="A1:B5"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937C09E1-B7DE-43A8-9BE4-32A1FF40797D}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" style="2" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2">
-        <v>7890</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4A8E5C-EBDF-47DF-A86D-8BC540B150E9}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="24.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{34139DEB-620A-4303-A065-72BFF66BD05A}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{6E73A26A-7715-4B11-A3B5-C1FB1D66628B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
naming convertions with all the assertions
</commit_message>
<xml_diff>
--- a/testdata/data.xlsx
+++ b/testdata/data.xlsx
@@ -3,27 +3,41 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{86AC9050-8644-4529-9235-71738283DB54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A9BED9-2015-4F05-BC56-4E874A6ABFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4B24D542-0957-4B90-AF3B-FDAF134FB36C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{4B24D542-0957-4B90-AF3B-FDAF134FB36C}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="validlogin" sheetId="2" r:id="rId2"/>
     <sheet name="register" sheetId="3" r:id="rId3"/>
+    <sheet name="code" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:L5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>z</t>
   </si>
@@ -40,9 +54,6 @@
     <t xml:space="preserve"> Please fill out this field </t>
   </si>
   <si>
-    <t>r</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -65,6 +76,30 @@
   </si>
   <si>
     <t>asdfew</t>
+  </si>
+  <si>
+    <t>abcdef</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>please fill out this field</t>
+  </si>
+  <si>
+    <t>missmathch password</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>printabc</t>
+  </si>
+  <si>
+    <t>print'Hello'</t>
   </si>
 </sst>
 </file>
@@ -432,7 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934FCFEA-8BD1-498C-B296-8BAE571437A6}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -461,7 +496,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -469,7 +504,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -477,13 +512,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -513,24 +548,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -545,15 +580,118 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937C09E1-B7DE-43A8-9BE4-32A1FF40797D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{7BB29354-E6F7-4A23-9859-4E9B3F637F04}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{3738AE72-0536-4461-B3B0-437463FD55DB}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{D8B9D3C0-2DB4-47E5-AEDC-ACB9363B1CD2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4828BA52-A60B-48A3-BA6E-2038D4BF3B24}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>